<commit_message>
Updated files for crab catch estimation
Removed line # 519 from summer and winter function. Updated folders with 2023 CRC winter data.
</commit_message>
<xml_diff>
--- a/CRC Data/CRC Reporting Rates/CRC_Reporting_Rates.xlsx
+++ b/CRC Data/CRC Reporting Rates/CRC_Reporting_Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFPCrustyAll/Shared Documents/Recreational Fisheries/Catch Memos/CRC Data Analysis Blair W/CRC Data/CRC Reporting Rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE68D657-C911-4D83-8A9B-E40E98CE998C}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{051FDBBF-4EB5-4490-9768-799B2DE88F3A}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="948" windowWidth="16104" windowHeight="11112" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
+    <workbookView xWindow="240" yWindow="192" windowWidth="17160" windowHeight="12036" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04C9482-2E0A-4207-A50E-B1EBB04F5E66}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,6 +712,12 @@
       <c r="C18">
         <v>81947</v>
       </c>
+      <c r="D18">
+        <v>32975</v>
+      </c>
+      <c r="E18">
+        <v>15204</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -719,17 +725,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="62120a19-a38a-4c78-8e86-03b65bdcf4fa">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE9114A9D0DECB469CD3434F7556ACE4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="69096168ac7ced0b799f829a42a3dc95">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="62120a19-a38a-4c78-8e86-03b65bdcf4fa" xmlns:ns3="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cc6a4a317e1aa101042744f0dc04384" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE9114A9D0DECB469CD3434F7556ACE4" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ecdf13fd03e578e190d1c2fef808890a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="62120a19-a38a-4c78-8e86-03b65bdcf4fa" xmlns:ns3="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d204db95074059abcc46212eb5d192a9" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="62120a19-a38a-4c78-8e86-03b65bdcf4fa"/>
     <xsd:import namespace="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d"/>
@@ -755,6 +765,7 @@
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -836,6 +847,11 @@
     <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="24" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -979,16 +995,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39DF0C60-8600-4ABA-BCDA-512E931CADE7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1BC7CAC-2F04-4EBF-9276-556CFC88EAC6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="671c5c8a-d1dd-40a7-bcfd-3ed591bedb5d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="62120a19-a38a-4c78-8e86-03b65bdcf4fa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3156BA-14FA-49D3-87A2-A352F4EC701D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{054E103B-5DB1-4C20-8F5C-86EDDFB12D70}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1005,4 +1034,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39DF0C60-8600-4ABA-BCDA-512E931CADE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated reporting rate file
This file included the summer 2024 reporting rates based on WildIDs.
</commit_message>
<xml_diff>
--- a/CRC Data/CRC Reporting Rates/CRC_Reporting_Rates.xlsx
+++ b/CRC Data/CRC Reporting Rates/CRC_Reporting_Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFPCrustyAll/Shared Documents/Recreational Fisheries/Catch Memos/CRC Data Analysis Blair W/CRC Data/CRC Reporting Rates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFPCrustyAll/Shared Documents/Recreational Fisheries/Catch Memos/CRC Data Analysis/CRC Data/CRC Estimate Function Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{051FDBBF-4EB5-4490-9768-799B2DE88F3A}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{AC9D3338-A214-49F3-A0F5-015DC57AFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F23AC27-10CF-4D0F-AEE4-E5AF6EF7B600}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="192" windowWidth="17160" windowHeight="12036" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
+    <workbookView xWindow="8064" yWindow="612" windowWidth="14688" windowHeight="9576" xr2:uid="{419BAF26-5BC6-4352-9EBC-5A6389D0E4C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,16 +41,16 @@
     <t>yr.vec</t>
   </si>
   <si>
-    <t>total.crc.winter</t>
+    <t>total.crc.Summer</t>
   </si>
   <si>
-    <t>reported.crc.winter</t>
+    <t>reported.crc.Summer</t>
   </si>
   <si>
-    <t>total.crc.summer</t>
+    <t>total.crc.Winter</t>
   </si>
   <si>
-    <t>reported.crc.summer</t>
+    <t>reported.crc.Winter</t>
   </si>
 </sst>
 </file>
@@ -402,15 +402,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04C9482-2E0A-4207-A50E-B1EBB04F5E66}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -418,16 +421,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -717,6 +720,17 @@
       </c>
       <c r="E18">
         <v>15204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2024</v>
+      </c>
+      <c r="B19">
+        <v>187214</v>
+      </c>
+      <c r="C19">
+        <v>81091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>